<commit_message>
lots of things working now, a few to go
</commit_message>
<xml_diff>
--- a/public/templates/occurrences.xlsx
+++ b/public/templates/occurrences.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
-    <t>dateLastModified</t>
+    <t>modified</t>
   </si>
   <si>
     <t>institutionCode</t>
@@ -104,26 +104,26 @@
   </numFmts>
   <fonts count="4">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,7 +193,7 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K48" activeCellId="0" pane="topLeft" sqref="K48:L48"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>

</xml_diff>